<commit_message>
Saving changes in Readme.xlsx and MiP_WUR_particles
</commit_message>
<xml_diff>
--- a/MINAGRIS_Plastic.R_ReadMe.xlsx
+++ b/MINAGRIS_Plastic.R_ReadMe.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\WURNET.NL\Homes\berio001\My Documents\R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berio001\Minagris\MINAGRIS_Microplastic_Soil_Assessmnent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E9C982-EC70-4291-804B-D9464EAF1247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5ADBF8C-6D6A-4884-9C83-A76C75966CBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14385" yWindow="-21600" windowWidth="24180" windowHeight="21000" xr2:uid="{A634431C-1F0B-4477-A9DD-2C46E099AE2B}"/>
+    <workbookView xWindow="-13155" yWindow="-21720" windowWidth="51840" windowHeight="21240" xr2:uid="{A634431C-1F0B-4477-A9DD-2C46E099AE2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Scripts" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="179">
   <si>
     <t>MINAGRIS_MiP_Summerize.R</t>
   </si>
@@ -561,6 +561,21 @@
   </si>
   <si>
     <t>Broken</t>
+  </si>
+  <si>
+    <t>MINAGRIS_MiP_WUR_Check_RawData.R</t>
+  </si>
+  <si>
+    <t>Check the raw data from WUR and extract names</t>
+  </si>
+  <si>
+    <t>WUR uFTIR raw data folders structure</t>
+  </si>
+  <si>
+    <t>Table of raw data available</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To be written </t>
   </si>
 </sst>
 </file>
@@ -706,7 +721,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -764,6 +779,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1083,10 +1101,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF91BE61-BE6D-498E-8510-3ABC584357F6}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1125,36 +1143,34 @@
     </row>
     <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>176</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>177</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>31</v>
@@ -1163,141 +1179,161 @@
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>40</v>
+        <v>21</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>31</v>
+        <v>39</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="D7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E8" s="7"/>
-    </row>
-    <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F10" s="9" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+    <row r="11" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>29</v>
       </c>
     </row>
+    <row r="12" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{5CE255C4-890B-4C8B-A7EA-4A78990DDE0E}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{999A6839-A363-4B9F-AA3D-17483B5AB2E9}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{EC5FCA71-9DCB-435D-87E5-C178CBCF0ACE}"/>
-    <hyperlink ref="F5" r:id="rId4" xr:uid="{11BA7B88-988D-4E04-98D5-6E8312C0D113}"/>
-    <hyperlink ref="F9" r:id="rId5" xr:uid="{53ECD34B-AB2F-4F42-B79F-E2E722C1433F}"/>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{5CE255C4-890B-4C8B-A7EA-4A78990DDE0E}"/>
+    <hyperlink ref="F4" r:id="rId2" xr:uid="{999A6839-A363-4B9F-AA3D-17483B5AB2E9}"/>
+    <hyperlink ref="F5" r:id="rId3" xr:uid="{EC5FCA71-9DCB-435D-87E5-C178CBCF0ACE}"/>
+    <hyperlink ref="F6" r:id="rId4" xr:uid="{11BA7B88-988D-4E04-98D5-6E8312C0D113}"/>
+    <hyperlink ref="F10" r:id="rId5" xr:uid="{53ECD34B-AB2F-4F42-B79F-E2E722C1433F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Common order of use of the scripts added in ReadMe
</commit_message>
<xml_diff>
--- a/MINAGRIS_Plastic.R_ReadMe.xlsx
+++ b/MINAGRIS_Plastic.R_ReadMe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berio001\Minagris\MINAGRIS_Microplastic_Soil_Assessmnent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9CF2F03-53D4-4AB7-919C-8D45812022D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0716964C-9929-47C0-9FAF-ECA2A132CE77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16395" yWindow="-21600" windowWidth="22170" windowHeight="21000" xr2:uid="{A634431C-1F0B-4477-A9DD-2C46E099AE2B}"/>
   </bookViews>
@@ -1117,7 +1117,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1159,7 +1159,9 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="25"/>
+      <c r="A2" s="25">
+        <v>1</v>
+      </c>
       <c r="B2" s="3" t="s">
         <v>172</v>
       </c>
@@ -1180,6 +1182,9 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>4</v>
+      </c>
       <c r="B3" s="3" t="s">
         <v>173</v>
       </c>
@@ -1193,6 +1198,9 @@
       <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>5</v>
+      </c>
       <c r="B4" s="3" t="s">
         <v>178</v>
       </c>
@@ -1207,6 +1215,9 @@
       <c r="G4" s="8"/>
     </row>
     <row r="5" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
       <c r="B5" s="3" t="s">
         <v>26</v>
       </c>
@@ -1227,6 +1238,9 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>3</v>
+      </c>
       <c r="B6" s="3" t="s">
         <v>32</v>
       </c>
@@ -1247,6 +1261,9 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
       <c r="B7" s="3" t="s">
         <v>0</v>
       </c>
@@ -1267,6 +1284,9 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
       <c r="B8" s="3" t="s">
         <v>1</v>
       </c>
@@ -1304,6 +1324,9 @@
       <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>8</v>
+      </c>
       <c r="B11" s="3" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
MINAGRIS_MiP_Summerize.R divided into first MINAGRIS_MiP_Correction and then MINAGRIS_MiP_Summerize.R
Add a Matching quality threshold of 0.35 for "other plastics" in MINAGRIS_MiP_Correction
</commit_message>
<xml_diff>
--- a/MINAGRIS_Plastic.R_ReadMe.xlsx
+++ b/MINAGRIS_Plastic.R_ReadMe.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berio001\Minagris\MINAGRIS_Microplastic_Soil_Assessmnent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0716964C-9929-47C0-9FAF-ECA2A132CE77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{824825E2-A76E-4647-96C1-3D4E052AB2CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16395" yWindow="-21600" windowWidth="22170" windowHeight="21000" xr2:uid="{A634431C-1F0B-4477-A9DD-2C46E099AE2B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A634431C-1F0B-4477-A9DD-2C46E099AE2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Scripts" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="184">
   <si>
     <t>MINAGRIS_MiP_Summerize.R</t>
   </si>
@@ -102,9 +102,6 @@
   </si>
   <si>
     <t>Corrected_MiP_Particles_date.csv, MeP_Particles_date.csv, MaP_Particles_date.csv,</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Load result table from Ubern and WUR ; Merge data of both labs ; Blank correction ; Mass estimation ; Make summary table of any kind ; create size categories </t>
   </si>
   <si>
     <t>MiP.MeP.MaP_META_date.csv</t>
@@ -567,9 +564,6 @@
     <t>Check the available raw data from WUR and create IR data  METADATA</t>
   </si>
   <si>
-    <t xml:space="preserve">To be checked </t>
-  </si>
-  <si>
     <t>IR_METADATA_2024.11.13.csv IR_SummaryCSS_2024.11.13.csv IR_SummaryQC_2024.11.13.csv</t>
   </si>
   <si>
@@ -586,6 +580,18 @@
   </si>
   <si>
     <t>Check the processed and visually checked results (PMF data) from WUR, create METADATA, combined result table and Correct the scale of px size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Working, to be checked </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Load result table from Ubern and WUR ; Merge data of both labs ; Blank correction ; Mass estimation ; Make summary table of any kind ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Load result table from Ubern and WUR ; Merge data of both labs ; Blank correction ; Mass estimation ; "Other plastic correction"  create size categories </t>
+  </si>
+  <si>
+    <t>MINAGRIS_MiP_Correction</t>
   </si>
 </sst>
 </file>
@@ -1114,10 +1120,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF91BE61-BE6D-498E-8510-3ABC584357F6}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1134,7 +1140,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>10</v>
@@ -1152,10 +1158,10 @@
         <v>12</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -1163,112 +1169,115 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C2" s="24" t="s">
+        <v>173</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="E2" s="24" t="s">
         <v>174</v>
       </c>
-      <c r="D2" s="24" t="s">
-        <v>170</v>
-      </c>
-      <c r="E2" s="24" t="s">
-        <v>176</v>
-      </c>
       <c r="F2" s="4" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>181</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="24" t="s">
+      <c r="D3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="G3" s="8"/>
+      <c r="G3" s="9" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>179</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="G4" s="8"/>
+        <v>31</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>17</v>
+        <v>172</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>179</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="24" t="s">
+        <v>178</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>180</v>
+      </c>
+      <c r="G5" s="8"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>168</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>177</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>21</v>
+        <v>183</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>182</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>18</v>
@@ -1276,113 +1285,131 @@
       <c r="E7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="F7" s="7"/>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="B9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="F10" s="7"/>
+      <c r="E9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="1">
-        <v>8</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>3</v>
+      <c r="B11" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="9" t="s">
+      <c r="F11" s="23" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B12" s="3" t="s">
+      <c r="G11" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="B13" s="3" t="s">
+      <c r="E13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="B14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>25</v>
+      <c r="D14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H14">
+    <sortCondition ref="A2:A14"/>
+  </sortState>
   <hyperlinks>
-    <hyperlink ref="G5" r:id="rId1" xr:uid="{999A6839-A363-4B9F-AA3D-17483B5AB2E9}"/>
-    <hyperlink ref="G6" r:id="rId2" xr:uid="{EC5FCA71-9DCB-435D-87E5-C178CBCF0ACE}"/>
-    <hyperlink ref="G7" r:id="rId3" xr:uid="{11BA7B88-988D-4E04-98D5-6E8312C0D113}"/>
-    <hyperlink ref="G11" r:id="rId4" xr:uid="{53ECD34B-AB2F-4F42-B79F-E2E722C1433F}"/>
+    <hyperlink ref="G3" r:id="rId1" xr:uid="{999A6839-A363-4B9F-AA3D-17483B5AB2E9}"/>
+    <hyperlink ref="G4" r:id="rId2" xr:uid="{EC5FCA71-9DCB-435D-87E5-C178CBCF0ACE}"/>
+    <hyperlink ref="G8" r:id="rId3" xr:uid="{11BA7B88-988D-4E04-98D5-6E8312C0D113}"/>
+    <hyperlink ref="G10" r:id="rId4" xr:uid="{53ECD34B-AB2F-4F42-B79F-E2E722C1433F}"/>
     <hyperlink ref="G2" r:id="rId5" xr:uid="{80B183D0-3023-49BE-A6E8-A403454024A3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1407,149 +1434,149 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>40</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="C2" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="D2" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="E2" s="13" t="s">
         <v>45</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="D3" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="E3" s="13" t="s">
         <v>45</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="D4" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="E4" s="13" t="s">
         <v>45</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="C5" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="D5" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>52</v>
-      </c>
       <c r="E5" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="C6" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="D6" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="E6" s="13" t="s">
         <v>56</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="C7" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="D7" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="E7" s="13" t="s">
         <v>61</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="C8" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="D8" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="E8" s="13" t="s">
         <v>66</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="C9" s="12" t="s">
         <v>69</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>70</v>
       </c>
       <c r="D9" s="13">
         <v>711</v>
@@ -1560,13 +1587,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="C10" s="12" t="s">
         <v>72</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>73</v>
       </c>
       <c r="D10" s="13">
         <v>7</v>
@@ -1577,13 +1604,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="C11" s="12" t="s">
         <v>75</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>76</v>
       </c>
       <c r="D11" s="13">
         <v>1</v>
@@ -1594,13 +1621,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="C12" s="12" t="s">
         <v>78</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>79</v>
       </c>
       <c r="D12" s="13">
         <v>1</v>
@@ -1611,115 +1638,115 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="C13" s="12" t="s">
         <v>81</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>82</v>
       </c>
       <c r="D13" s="13">
         <v>0</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="C14" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="D14" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="E14" s="13" t="s">
         <v>87</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="C15" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="D15" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" s="13" t="s">
         <v>91</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="C16" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="D16" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="E16" s="13" t="s">
         <v>96</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="C17" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="D17" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="13" t="s">
-        <v>101</v>
-      </c>
       <c r="E17" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="C18" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="D18" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="E18" s="13" t="s">
         <v>105</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="C19" s="12" t="s">
         <v>108</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>109</v>
       </c>
       <c r="D19" s="13">
         <v>756</v>
@@ -1730,13 +1757,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="C20" s="12" t="s">
         <v>111</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>112</v>
       </c>
       <c r="D20" s="13">
         <v>88.8</v>
@@ -1747,182 +1774,182 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="B21" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="B21" s="14" t="s">
-        <v>114</v>
-      </c>
       <c r="C21" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B22" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="B22" s="16" t="s">
-        <v>116</v>
-      </c>
       <c r="C22" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="B23" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="C23" s="16" t="s">
         <v>118</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>119</v>
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="B24" s="16" t="s">
-        <v>121</v>
-      </c>
       <c r="C24" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="B25" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="B25" s="16" t="s">
-        <v>123</v>
-      </c>
       <c r="C25" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D25" s="15"/>
       <c r="E25" s="15"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="B26" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="B26" s="16" t="s">
-        <v>125</v>
-      </c>
       <c r="C26" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D26" s="15"/>
       <c r="E26" s="15"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="B27" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="C27" s="16" t="s">
         <v>127</v>
-      </c>
-      <c r="C27" s="16" t="s">
-        <v>128</v>
       </c>
       <c r="D27" s="15"/>
       <c r="E27" s="15"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B28" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="B28" s="16" t="s">
-        <v>130</v>
-      </c>
       <c r="C28" s="16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D28" s="15"/>
       <c r="E28" s="15"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="B29" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="B29" s="16" t="s">
-        <v>132</v>
-      </c>
       <c r="C29" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D29" s="15"/>
       <c r="E29" s="15"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="B30" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="B30" s="16" t="s">
-        <v>134</v>
-      </c>
       <c r="C30" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D30" s="15"/>
       <c r="E30" s="15"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="B31" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="B31" s="16" t="s">
-        <v>136</v>
-      </c>
       <c r="C31" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D31" s="15"/>
       <c r="E31" s="15"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B32" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="B32" s="16" t="s">
-        <v>138</v>
-      </c>
       <c r="C32" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D32" s="15"/>
       <c r="E32" s="15"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="B33" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="B33" s="16" t="s">
+      <c r="C33" s="16" t="s">
         <v>140</v>
-      </c>
-      <c r="C33" s="16" t="s">
-        <v>141</v>
       </c>
       <c r="D33" s="15"/>
       <c r="E33" s="15"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B34" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="B34" s="16" t="s">
-        <v>143</v>
-      </c>
       <c r="C34" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D34" s="15"/>
       <c r="E34" s="15"/>
@@ -1951,115 +1978,115 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>11</v>
       </c>
       <c r="C1" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="E1" s="18" t="s">
         <v>40</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="C2" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="D2" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="E2" s="19" t="s">
         <v>45</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="C3" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="D3" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="19" t="s">
-        <v>52</v>
-      </c>
       <c r="E3" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="C4" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="D4" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="E4" s="19" t="s">
         <v>56</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="C5" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="D5" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="E5" s="15" t="s">
         <v>61</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="C6" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="D6" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="E6" s="19" t="s">
         <v>66</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="C7" s="16" t="s">
         <v>69</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>70</v>
       </c>
       <c r="D7" s="15">
         <v>711</v>
@@ -2070,13 +2097,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="C8" s="16" t="s">
         <v>72</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>73</v>
       </c>
       <c r="D8" s="15">
         <v>7</v>
@@ -2087,13 +2114,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="C9" s="16" t="s">
         <v>75</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>76</v>
       </c>
       <c r="D9" s="15">
         <v>1</v>
@@ -2104,13 +2131,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="C10" s="16" t="s">
         <v>78</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>79</v>
       </c>
       <c r="D10" s="15">
         <v>1</v>
@@ -2121,243 +2148,243 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="C11" s="16" t="s">
         <v>81</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>82</v>
       </c>
       <c r="D11" s="15">
         <v>0</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="C12" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="D12" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="E12" s="19" t="s">
         <v>87</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="C13" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="C13" s="16" t="s">
-        <v>91</v>
-      </c>
       <c r="D13" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E13" s="20"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="C14" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="D14" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="E14" s="20" t="s">
         <v>96</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="C15" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="D15" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="D15" s="20" t="s">
-        <v>101</v>
-      </c>
       <c r="E15" s="20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="B16" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="C16" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="D16" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="E16" s="20" t="s">
         <v>105</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B17" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="B17" s="16" t="s">
-        <v>114</v>
-      </c>
       <c r="C17" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B18" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="B18" s="16" t="s">
-        <v>116</v>
-      </c>
       <c r="C18" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D18" s="15"/>
       <c r="E18" s="15"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="B19" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="C19" s="16" t="s">
         <v>118</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>119</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="B20" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="B20" s="16" t="s">
-        <v>121</v>
-      </c>
       <c r="C20" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="B21" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="B21" s="16" t="s">
-        <v>123</v>
-      </c>
       <c r="C21" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="B22" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="B22" s="16" t="s">
-        <v>145</v>
-      </c>
       <c r="C22" s="16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="B23" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="B23" s="16" t="s">
-        <v>134</v>
-      </c>
       <c r="C23" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="B24" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="B24" s="16" t="s">
-        <v>136</v>
-      </c>
       <c r="C24" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B25" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="B25" s="16" t="s">
-        <v>138</v>
-      </c>
       <c r="C25" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D25" s="15"/>
       <c r="E25" s="15"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="B26" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="C26" s="16" t="s">
         <v>140</v>
-      </c>
-      <c r="C26" s="16" t="s">
-        <v>141</v>
       </c>
       <c r="D26" s="15"/>
       <c r="E26" s="15"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B27" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="B27" s="16" t="s">
-        <v>143</v>
-      </c>
       <c r="C27" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D27" s="15"/>
       <c r="E27" s="15"/>
@@ -2383,13 +2410,13 @@
   <sheetData>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="B5" s="21" t="s">
         <v>161</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="C5" s="21" t="s">
         <v>162</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -2397,10 +2424,10 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -2408,10 +2435,10 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -2419,10 +2446,10 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -2430,10 +2457,10 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -2441,10 +2468,10 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -2452,42 +2479,42 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="22" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="22" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="C16" t="s">
         <v>166</v>
-      </c>
-      <c r="C16" t="s">
-        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Visualize updated with graphs of all CSS and all polymers
</commit_message>
<xml_diff>
--- a/MINAGRIS_Plastic.R_ReadMe.xlsx
+++ b/MINAGRIS_Plastic.R_ReadMe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berio001\Minagris\MINAGRIS_Microplastic_Soil_Assessmnent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{824825E2-A76E-4647-96C1-3D4E052AB2CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38FA87F5-8BCE-4133-998C-300322BFB71B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A634431C-1F0B-4477-A9DD-2C46E099AE2B}"/>
   </bookViews>
@@ -1123,7 +1123,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
New plotting of the Bar graphs: Average per Field
</commit_message>
<xml_diff>
--- a/MINAGRIS_Plastic.R_ReadMe.xlsx
+++ b/MINAGRIS_Plastic.R_ReadMe.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berio001\Documents\MINAGRIS_C\MINAGRIS_Microplastic_Soil_Assessmnent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A7902F-C94F-4D16-A914-D7FE709506A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C818A5DA-0D04-47EA-BF8A-DDA7CC11F532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11670" yWindow="-21720" windowWidth="51840" windowHeight="21120" xr2:uid="{A634431C-1F0B-4477-A9DD-2C46E099AE2B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="3" xr2:uid="{A634431C-1F0B-4477-A9DD-2C46E099AE2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Scripts" sheetId="1" r:id="rId1"/>
     <sheet name="WUR Data" sheetId="2" r:id="rId2"/>
     <sheet name="Merged WUR Ubern data" sheetId="3" r:id="rId3"/>
     <sheet name="Summaries" sheetId="4" r:id="rId4"/>
+    <sheet name="Replicated soils in IR files " sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="229">
   <si>
     <t>MINAGRIS_MiP_Summerize.R</t>
   </si>
@@ -634,13 +635,106 @@
   </si>
   <si>
     <t>summary tables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.6.1_S1   6.1.1_S1   8.1.2_S1   8.3.1_S1   8.3.2_S1   8.5.2_S1   8.6.1_S1   8.6.2_S1   8.7.2_S1   8.8.1_S1   9.4.2_S1 11.10.2_S1 11.10.1_S1  11.4.1_S2   1.2.1_S2  5.10.2_S2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         2          2          2          2          2          2          2          2          2          2          2          4          6          7          9         10</t>
+  </si>
+  <si>
+    <t>3.6.1_S1</t>
+  </si>
+  <si>
+    <t>6.1.1_S1</t>
+  </si>
+  <si>
+    <t>8.1.2_S1</t>
+  </si>
+  <si>
+    <t>8.3.1_S1</t>
+  </si>
+  <si>
+    <t>8.3.2_S1</t>
+  </si>
+  <si>
+    <t>8.5.2_S1</t>
+  </si>
+  <si>
+    <t>8.6.1_S1</t>
+  </si>
+  <si>
+    <t>8.6.2_S1</t>
+  </si>
+  <si>
+    <t>8.7.2_S1</t>
+  </si>
+  <si>
+    <t>8.8.1_S1</t>
+  </si>
+  <si>
+    <t>9.4.2_S1</t>
+  </si>
+  <si>
+    <t>11.10.2_S1</t>
+  </si>
+  <si>
+    <t>11.10.1_S1</t>
+  </si>
+  <si>
+    <t>11.4.1_S2</t>
+  </si>
+  <si>
+    <t>1.2.1_S2</t>
+  </si>
+  <si>
+    <t>5.10.2_S2</t>
+  </si>
+  <si>
+    <t>1.6.1_S1</t>
+  </si>
+  <si>
+    <t>7.1.1_S2</t>
+  </si>
+  <si>
+    <t>7.1.1_S1</t>
+  </si>
+  <si>
+    <t>9.9.2_S1</t>
+  </si>
+  <si>
+    <t>4.5.1_S1</t>
+  </si>
+  <si>
+    <t>rs</t>
+  </si>
+  <si>
+    <t>st</t>
+  </si>
+  <si>
+    <t>bcm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n IR Files </t>
+  </si>
+  <si>
+    <t>Soil Samle</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>Polymer.red3 * Size_cat.um</t>
+  </si>
+  <si>
+    <t>i</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -687,6 +781,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -811,7 +912,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -882,6 +983,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="3" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1202,7 +1304,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF91BE61-BE6D-498E-8510-3ABC584357F6}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
@@ -2078,7 +2180,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2510,10 +2612,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{974A020C-A60C-4913-8965-C046DA9F3A39}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2610,60 +2712,486 @@
         <v>177</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="C10" t="s">
-        <v>178</v>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="18">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C11" t="s">
-        <v>156</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C12" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C13" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="C14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="C15" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="C16" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="18" t="s">
         <v>182</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>183</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="C18" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="C19" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9F5E76E-42C8-413A-AD46-C3B4D0333999}">
+  <dimension ref="B4:Z42"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:C42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>200</v>
+      </c>
+      <c r="D4" t="s">
+        <v>201</v>
+      </c>
+      <c r="E4" t="s">
+        <v>202</v>
+      </c>
+      <c r="F4" t="s">
+        <v>203</v>
+      </c>
+      <c r="G4" t="s">
+        <v>204</v>
+      </c>
+      <c r="H4" t="s">
+        <v>205</v>
+      </c>
+      <c r="I4" t="s">
+        <v>206</v>
+      </c>
+      <c r="J4" t="s">
+        <v>207</v>
+      </c>
+      <c r="K4" t="s">
+        <v>208</v>
+      </c>
+      <c r="L4" t="s">
+        <v>209</v>
+      </c>
+      <c r="M4" t="s">
+        <v>210</v>
+      </c>
+      <c r="N4" t="s">
+        <v>211</v>
+      </c>
+      <c r="O4" t="s">
+        <v>212</v>
+      </c>
+      <c r="P4" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>214</v>
+      </c>
+      <c r="R4" t="s">
+        <v>215</v>
+      </c>
+      <c r="S4" t="s">
+        <v>216</v>
+      </c>
+      <c r="T4" t="s">
+        <v>217</v>
+      </c>
+      <c r="U4" t="s">
+        <v>218</v>
+      </c>
+      <c r="V4" t="s">
+        <v>219</v>
+      </c>
+      <c r="W4" t="s">
+        <v>220</v>
+      </c>
+      <c r="X4" t="s">
+        <v>221</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>222</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="5" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="N5">
+        <v>4</v>
+      </c>
+      <c r="O5">
+        <v>6</v>
+      </c>
+      <c r="P5">
+        <v>7</v>
+      </c>
+      <c r="Q5">
+        <v>9</v>
+      </c>
+      <c r="R5">
+        <v>10</v>
+      </c>
+      <c r="S5">
+        <v>11</v>
+      </c>
+      <c r="T5">
+        <v>11</v>
+      </c>
+      <c r="U5">
+        <v>12</v>
+      </c>
+      <c r="V5">
+        <v>13</v>
+      </c>
+      <c r="W5">
+        <v>14</v>
+      </c>
+      <c r="X5">
+        <v>18</v>
+      </c>
+      <c r="Y5">
+        <v>41</v>
+      </c>
+      <c r="Z5">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="F10" t="s">
+        <v>216</v>
+      </c>
+      <c r="G10" t="s">
+        <v>217</v>
+      </c>
+      <c r="H10" t="s">
+        <v>218</v>
+      </c>
+      <c r="I10" t="s">
+        <v>219</v>
+      </c>
+      <c r="J10" t="s">
+        <v>220</v>
+      </c>
+      <c r="K10" t="s">
+        <v>221</v>
+      </c>
+      <c r="L10" t="s">
+        <v>222</v>
+      </c>
+      <c r="M10" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="11" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="12" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>225</v>
+      </c>
+      <c r="C18" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>200</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>201</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>202</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>203</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>204</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>205</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>206</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>207</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>208</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>209</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>210</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B30" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="C30" s="28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B31" s="28" t="s">
+        <v>212</v>
+      </c>
+      <c r="C31" s="28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>213</v>
+      </c>
+      <c r="C32">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>214</v>
+      </c>
+      <c r="C33">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>215</v>
+      </c>
+      <c r="C34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>217</v>
+      </c>
+      <c r="C36">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>218</v>
+      </c>
+      <c r="C37">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>219</v>
+      </c>
+      <c r="C38">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>220</v>
+      </c>
+      <c r="C39">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>221</v>
+      </c>
+      <c r="C40">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>222</v>
+      </c>
+      <c r="C41">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>223</v>
+      </c>
+      <c r="C42">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Field MetaData added in the analysis
</commit_message>
<xml_diff>
--- a/MINAGRIS_Plastic.R_ReadMe.xlsx
+++ b/MINAGRIS_Plastic.R_ReadMe.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berio001\Documents\MINAGRIS_C\MINAGRIS_Microplastic_Soil_Assessmnent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C818A5DA-0D04-47EA-BF8A-DDA7CC11F532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1CD5939-D0AD-4402-9319-E85AC65AA96C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="3" xr2:uid="{A634431C-1F0B-4477-A9DD-2C46E099AE2B}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" firstSheet="2" activeTab="4" xr2:uid="{A634431C-1F0B-4477-A9DD-2C46E099AE2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Scripts" sheetId="1" r:id="rId1"/>
     <sheet name="WUR Data" sheetId="2" r:id="rId2"/>
-    <sheet name="Merged WUR Ubern data" sheetId="3" r:id="rId3"/>
-    <sheet name="Summaries" sheetId="4" r:id="rId4"/>
-    <sheet name="Replicated soils in IR files " sheetId="5" r:id="rId5"/>
+    <sheet name="Merged WUR Ubern data columns" sheetId="3" r:id="rId3"/>
+    <sheet name="Summaries_names" sheetId="4" r:id="rId4"/>
+    <sheet name="Summaries columns" sheetId="7" r:id="rId5"/>
+    <sheet name="Replicated soils in IR files " sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="270">
   <si>
     <t>MINAGRIS_MiP_Summerize.R</t>
   </si>
@@ -451,12 +452,6 @@
   </si>
   <si>
     <t xml:space="preserve">Associated size category </t>
-  </si>
-  <si>
-    <t>Area,</t>
-  </si>
-  <si>
-    <t>Measured Area</t>
   </si>
   <si>
     <t>a</t>
@@ -637,12 +632,6 @@
     <t>summary tables</t>
   </si>
   <si>
-    <t xml:space="preserve">3.6.1_S1   6.1.1_S1   8.1.2_S1   8.3.1_S1   8.3.2_S1   8.5.2_S1   8.6.1_S1   8.6.2_S1   8.7.2_S1   8.8.1_S1   9.4.2_S1 11.10.2_S1 11.10.1_S1  11.4.1_S2   1.2.1_S2  5.10.2_S2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">         2          2          2          2          2          2          2          2          2          2          2          4          6          7          9         10</t>
-  </si>
-  <si>
     <t>3.6.1_S1</t>
   </si>
   <si>
@@ -728,6 +717,141 @@
   </si>
   <si>
     <t>i</t>
+  </si>
+  <si>
+    <t>length.um</t>
+  </si>
+  <si>
+    <t>Width.um</t>
+  </si>
+  <si>
+    <t>Aspect_ratio</t>
+  </si>
+  <si>
+    <t>Mass_ng</t>
+  </si>
+  <si>
+    <t>Batch_Name</t>
+  </si>
+  <si>
+    <t>Matching Quality Index (Ubern: "rsq" ; WUR: "Relevance" (could also be "similarity"))</t>
+  </si>
+  <si>
+    <t>Associated size category ("90-300", "300-510", "510-720", "720-930", "930-1140", "1140-1350")</t>
+  </si>
+  <si>
+    <t>"CSS_Farm_Field"</t>
+  </si>
+  <si>
+    <t>CSS_Farm_Field</t>
+  </si>
+  <si>
+    <t>"CSS_Farm_Field" number for field samples, "Other"  for the rest</t>
+  </si>
+  <si>
+    <t>7_1_1</t>
+  </si>
+  <si>
+    <t>11_1_1</t>
+  </si>
+  <si>
+    <t>[-1:11]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSS number, -1 for others </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Farm number, -1 for others </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Field number, -1 for others </t>
+  </si>
+  <si>
+    <t>[-1:12]</t>
+  </si>
+  <si>
+    <t>[-1:4]</t>
+  </si>
+  <si>
+    <t>Mean.particles.CSS</t>
+  </si>
+  <si>
+    <t>Median.particles.CSS</t>
+  </si>
+  <si>
+    <t>Min.particles.CSS</t>
+  </si>
+  <si>
+    <t>Max.particles.CSS</t>
+  </si>
+  <si>
+    <t>Mean.px.CSS</t>
+  </si>
+  <si>
+    <t>Mean.Tot.Area.mm2.CSS</t>
+  </si>
+  <si>
+    <t>Median.Tot.Area.mm2.CSS</t>
+  </si>
+  <si>
+    <t>Min.Tot.Area.mm2.CSS</t>
+  </si>
+  <si>
+    <t>Max.Tot.Area.mm2.CSS</t>
+  </si>
+  <si>
+    <t>Mean.Tot.Mass.ng.CSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mean number of particle in 5g soil, per CSS </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Median number of particle in 5g soil, per CSS </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Min number of particle in 5g soil, per CSS </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Max number of particle in 5g soil, per CSS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean number of identified pixels in 5g soil, per CSS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean of the sum of identified plastic area in 5g soil, per CSS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Median of the sum of identified plastic area in 5g soil, per CSS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min of the sum of identified plastic area in 5g soil, per CSS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max of the sum of identified plastic area in 5g soil, per CSS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean of the sum of estimated identified plastic mass in 5g soil, per CSS </t>
+  </si>
+  <si>
+    <t>character string</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>"M#Number"</t>
+  </si>
+  <si>
+    <t>Inputs</t>
+  </si>
+  <si>
+    <t>"Batch"_"Soil_sample"_"Sample_type"_"Filter_div"</t>
+  </si>
+  <si>
+    <t>"Batch"_"Soil_sample"_"Sample_type"</t>
+  </si>
+  <si>
+    <t>[mm2]</t>
   </si>
 </sst>
 </file>
@@ -833,7 +957,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -871,26 +995,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -910,9 +1014,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -945,13 +1049,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -974,16 +1071,18 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="4" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="4" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="3" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1006,9 +1105,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1046,7 +1145,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1152,7 +1251,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1294,7 +1393,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1304,7 +1403,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF91BE61-BE6D-498E-8510-3ABC584357F6}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
@@ -1320,8 +1419,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
-        <v>162</v>
+      <c r="A1" s="18" t="s">
+        <v>160</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>10</v>
@@ -1343,60 +1442,60 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="21">
+      <c r="A2" s="18">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="C2" s="20" t="s">
-        <v>165</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>166</v>
+      <c r="D2" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>164</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>171</v>
+        <v>162</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>169</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>170</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>167</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="25" t="s">
-        <v>167</v>
+      <c r="E4" s="17"/>
+      <c r="F4" s="22" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1404,10 +1503,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>173</v>
+        <v>172</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>171</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>17</v>
@@ -1416,7 +1515,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1427,19 +1526,19 @@
         <v>0</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1459,7 +1558,7 @@
         <v>21</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1478,8 +1577,8 @@
       <c r="E8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="25" t="s">
-        <v>181</v>
+      <c r="F8" s="22" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1495,7 +1594,7 @@
       <c r="E9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="23" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1509,18 +1608,18 @@
       <c r="D10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="26" t="s">
+      <c r="F10" s="23" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
+    <row r="12" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="22" t="s">
-        <v>190</v>
+      <c r="A13" s="19" t="s">
+        <v>188</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>10</v>
@@ -1555,7 +1654,7 @@
         <v>16</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -1572,34 +1671,34 @@
         <v>29</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="F16" s="27"/>
+        <v>191</v>
+      </c>
+      <c r="F16" s="24"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="26" t="s">
-        <v>181</v>
+      <c r="F17" s="23" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>25</v>
@@ -1607,8 +1706,8 @@
       <c r="D18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="19" t="s">
-        <v>160</v>
+      <c r="F18" s="16" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -1624,7 +1723,7 @@
   <dimension ref="B1:F35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1875,13 +1974,13 @@
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>186</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>188</v>
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
@@ -2177,433 +2276,548 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21B06D6A-171C-4116-9E54-CCF83806DB95}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="B1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="64.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="71.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" customWidth="1"/>
+    <col min="3" max="3" width="64.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="28.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="C1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="E1" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="G1" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B2" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="C2" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="D2" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="F2" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="G2" s="9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="C3" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="D3" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="F3" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="G3" s="9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="12" t="s">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="26" t="s">
+        <v>229</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="D4" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="9">
+        <v>711</v>
+      </c>
+      <c r="G7" s="9">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="F8" s="9">
+        <v>7</v>
+      </c>
+      <c r="G8" s="9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="F9" s="9">
+        <v>1</v>
+      </c>
+      <c r="G9" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="F10" s="9">
+        <v>1</v>
+      </c>
+      <c r="G10" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="26" t="s">
+        <v>233</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" s="9">
+        <v>0</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="26" t="s">
+        <v>184</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B16" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B18" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="E18" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="11">
-        <v>711</v>
-      </c>
-      <c r="E7" s="11">
-        <v>1111</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" s="11">
-        <v>7</v>
-      </c>
-      <c r="E8" s="11">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" s="11">
-        <v>1</v>
-      </c>
-      <c r="E9" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="D10" s="11">
-        <v>1</v>
-      </c>
-      <c r="E10" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="D11" s="11">
-        <v>0</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="E13" s="16"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B19" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="B18" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="C18" s="12" t="s">
+      <c r="C19" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="E19" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="12" t="s">
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B20" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="C20" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="D20" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="E20" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="C21" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="D21" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="E21" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="12" t="s">
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B22" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="C22" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="D22" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="E22" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="C22" s="12" t="s">
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B23" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B24" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="E24" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="B23" s="12" t="s">
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B25" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="C25" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="D25" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="E25" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="B24" s="12" t="s">
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B26" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C26" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="D26" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="E26" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="B25" s="12" t="s">
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B27" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="C27" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="D27" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="E27" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="B26" s="12" t="s">
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B28" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="C28" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="D28" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="E28" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="12" t="s">
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B29" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="B27" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="C27" s="12" t="s">
+      <c r="C29" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="E29" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2614,106 +2828,107 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{974A020C-A60C-4913-8965-C046DA9F3A39}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="65.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>154</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>155</v>
-      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="18">
+      <c r="A2" s="15">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="15">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="15">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>143</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C4" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="18">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="15">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>144</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C5" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="18">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="18">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>146</v>
-      </c>
-      <c r="C5" t="s">
-        <v>151</v>
-      </c>
-    </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="18">
+      <c r="A6" s="15">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>70</v>
       </c>
       <c r="C6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="18">
+      <c r="A7" s="15">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>64</v>
       </c>
       <c r="C7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="18">
+      <c r="A8" s="15">
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C8" t="s">
         <v>175</v>
       </c>
-      <c r="C8" t="s">
-        <v>177</v>
-      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="18">
+      <c r="A9" s="15">
         <v>8</v>
       </c>
       <c r="B9" t="s">
@@ -2721,72 +2936,72 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="C12" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C13" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="C14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="C15" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="C16" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="C12" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="C13" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="C14" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="C15" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="18" t="s">
-        <v>179</v>
-      </c>
-      <c r="C16" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="18" t="s">
-        <v>182</v>
-      </c>
       <c r="C17" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="18" t="s">
-        <v>226</v>
+      <c r="A18" s="15" t="s">
+        <v>222</v>
       </c>
       <c r="C18" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="18" t="s">
-        <v>228</v>
+      <c r="A19" s="15" t="s">
+        <v>224</v>
       </c>
       <c r="C19" t="s">
         <v>115</v>
@@ -2798,399 +3013,614 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9F5E76E-42C8-413A-AD46-C3B4D0333999}">
-  <dimension ref="B4:Z42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A65C4286-6995-4B1C-8EDD-8F561F25CBD8}">
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:C42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="67.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:26" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="26" t="s">
+        <v>229</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="26" t="s">
+        <v>233</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="26" t="s">
+        <v>184</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="12" t="s">
+        <v>249</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>134</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9F5E76E-42C8-413A-AD46-C3B4D0333999}">
+  <dimension ref="A1:B25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>198</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>199</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>200</v>
       </c>
-      <c r="D4" t="s">
+      <c r="B6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>201</v>
       </c>
-      <c r="E4" t="s">
+      <c r="B7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>202</v>
       </c>
-      <c r="F4" t="s">
+      <c r="B8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>203</v>
       </c>
-      <c r="G4" t="s">
+      <c r="B9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>204</v>
       </c>
-      <c r="H4" t="s">
+      <c r="B10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>205</v>
       </c>
-      <c r="I4" t="s">
+      <c r="B11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>206</v>
       </c>
-      <c r="J4" t="s">
+      <c r="B12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="25" t="s">
         <v>207</v>
       </c>
-      <c r="K4" t="s">
+      <c r="B13" s="25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="25" t="s">
         <v>208</v>
       </c>
-      <c r="L4" t="s">
+      <c r="B14" s="25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>209</v>
       </c>
-      <c r="M4" t="s">
+      <c r="B15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>210</v>
       </c>
-      <c r="N4" t="s">
+      <c r="B16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>211</v>
       </c>
-      <c r="O4" t="s">
+      <c r="B17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>212</v>
       </c>
-      <c r="P4" t="s">
+      <c r="B18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>213</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="B19">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>214</v>
       </c>
-      <c r="R4" t="s">
+      <c r="B20">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>215</v>
       </c>
-      <c r="S4" t="s">
+      <c r="B21">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>216</v>
       </c>
-      <c r="T4" t="s">
+      <c r="B22">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>217</v>
       </c>
-      <c r="U4" t="s">
+      <c r="B23">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>218</v>
       </c>
-      <c r="V4" t="s">
+      <c r="B24">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>219</v>
       </c>
-      <c r="W4" t="s">
-        <v>220</v>
-      </c>
-      <c r="X4" t="s">
-        <v>221</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>222</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="5" spans="3:26" x14ac:dyDescent="0.3">
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <v>2</v>
-      </c>
-      <c r="I5">
-        <v>2</v>
-      </c>
-      <c r="J5">
-        <v>2</v>
-      </c>
-      <c r="K5">
-        <v>2</v>
-      </c>
-      <c r="L5">
-        <v>2</v>
-      </c>
-      <c r="M5">
-        <v>2</v>
-      </c>
-      <c r="N5">
-        <v>4</v>
-      </c>
-      <c r="O5">
-        <v>6</v>
-      </c>
-      <c r="P5">
-        <v>7</v>
-      </c>
-      <c r="Q5">
-        <v>9</v>
-      </c>
-      <c r="R5">
-        <v>10</v>
-      </c>
-      <c r="S5">
-        <v>11</v>
-      </c>
-      <c r="T5">
-        <v>11</v>
-      </c>
-      <c r="U5">
-        <v>12</v>
-      </c>
-      <c r="V5">
-        <v>13</v>
-      </c>
-      <c r="W5">
-        <v>14</v>
-      </c>
-      <c r="X5">
-        <v>18</v>
-      </c>
-      <c r="Y5">
-        <v>41</v>
-      </c>
-      <c r="Z5">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="3:26" x14ac:dyDescent="0.3">
-      <c r="F10" t="s">
-        <v>216</v>
-      </c>
-      <c r="G10" t="s">
-        <v>217</v>
-      </c>
-      <c r="H10" t="s">
-        <v>218</v>
-      </c>
-      <c r="I10" t="s">
-        <v>219</v>
-      </c>
-      <c r="J10" t="s">
-        <v>220</v>
-      </c>
-      <c r="K10" t="s">
-        <v>221</v>
-      </c>
-      <c r="L10" t="s">
-        <v>222</v>
-      </c>
-      <c r="M10" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="11" spans="3:26" x14ac:dyDescent="0.3">
-      <c r="D11" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="12" spans="3:26" x14ac:dyDescent="0.3">
-      <c r="D12" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>225</v>
-      </c>
-      <c r="C18" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
-        <v>200</v>
-      </c>
-      <c r="C19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
-        <v>201</v>
-      </c>
-      <c r="C20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
-        <v>202</v>
-      </c>
-      <c r="C21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>203</v>
-      </c>
-      <c r="C22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
-        <v>204</v>
-      </c>
-      <c r="C23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
-        <v>205</v>
-      </c>
-      <c r="C24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
-        <v>206</v>
-      </c>
-      <c r="C25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
-        <v>207</v>
-      </c>
-      <c r="C26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
-        <v>208</v>
-      </c>
-      <c r="C27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
-        <v>209</v>
-      </c>
-      <c r="C28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
-        <v>210</v>
-      </c>
-      <c r="C29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B30" s="28" t="s">
-        <v>211</v>
-      </c>
-      <c r="C30" s="28">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B31" s="28" t="s">
-        <v>212</v>
-      </c>
-      <c r="C31" s="28">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B32" t="s">
-        <v>213</v>
-      </c>
-      <c r="C32">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B33" t="s">
-        <v>214</v>
-      </c>
-      <c r="C33">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B34" t="s">
-        <v>215</v>
-      </c>
-      <c r="C34">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B35" t="s">
-        <v>216</v>
-      </c>
-      <c r="C35">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B36" t="s">
-        <v>217</v>
-      </c>
-      <c r="C36">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
-        <v>218</v>
-      </c>
-      <c r="C37">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B38" t="s">
-        <v>219</v>
-      </c>
-      <c r="C38">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B39" t="s">
-        <v>220</v>
-      </c>
-      <c r="C39">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B40" t="s">
-        <v>221</v>
-      </c>
-      <c r="C40">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B41" t="s">
-        <v>222</v>
-      </c>
-      <c r="C41">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B42" t="s">
-        <v>223</v>
-      </c>
-      <c r="C42">
+      <c r="B25">
         <v>42</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates because of the Ubern calculation: - adding Filter_div (/!\ manual selection of samples in Ubern!) - harmonize all _Names to _names '-Visualize CSS11 Farm 10 - visualise per crop
</commit_message>
<xml_diff>
--- a/MINAGRIS_Plastic.R_ReadMe.xlsx
+++ b/MINAGRIS_Plastic.R_ReadMe.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berio001\Documents\MINAGRIS_C\MINAGRIS_Microplastic_Soil_Assessmnent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1CD5939-D0AD-4402-9319-E85AC65AA96C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0049E7-5A08-4A1A-B1ED-FE9C12FA2223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" firstSheet="2" activeTab="4" xr2:uid="{A634431C-1F0B-4477-A9DD-2C46E099AE2B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="2" activeTab="2" xr2:uid="{A634431C-1F0B-4477-A9DD-2C46E099AE2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Scripts" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="276">
   <si>
     <t>MINAGRIS_MiP_Summerize.R</t>
   </si>
@@ -572,9 +572,6 @@
     <t>Mean All MINAGRIS project</t>
   </si>
   <si>
-    <t>All factors: Polymer.grp, Polymer.red12,  Polymer.red3, Size_cat.um</t>
-  </si>
-  <si>
     <t>f</t>
   </si>
   <si>
@@ -852,6 +849,27 @@
   </si>
   <si>
     <t>[mm2]</t>
+  </si>
+  <si>
+    <t>Mean per farm</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>All factors: Polymer.grp, Polymer.red12,  Polymer.red3, Size_cat.um,  Size_cat2.um</t>
+  </si>
+  <si>
+    <t>Polymer.grp,  Polymer.red12,  Polymer.red3</t>
+  </si>
+  <si>
+    <t>Crop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Per dominant croping system </t>
   </si>
 </sst>
 </file>
@@ -1461,12 +1479,12 @@
         <v>170</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>162</v>
@@ -1484,7 +1502,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>166</v>
@@ -1526,19 +1544,19 @@
         <v>0</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>170</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1578,7 +1596,7 @@
         <v>22</v>
       </c>
       <c r="F8" s="22" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1619,7 +1637,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>10</v>
@@ -1676,29 +1694,29 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F16" s="24"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>25</v>
@@ -1974,13 +1992,13 @@
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="D15" s="8" t="s">
         <v>185</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>186</v>
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
@@ -2278,8 +2296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21B06D6A-171C-4116-9E54-CCF83806DB95}">
   <dimension ref="B1:G29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="E18:F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2302,7 +2320,7 @@
         <v>32</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>33</v>
@@ -2319,7 +2337,7 @@
         <v>36</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>37</v>
@@ -2339,7 +2357,7 @@
         <v>43</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>44</v>
@@ -2353,16 +2371,16 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" s="26" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>47</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>49</v>
@@ -2379,7 +2397,7 @@
         <v>52</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>53</v>
@@ -2399,7 +2417,7 @@
         <v>57</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>58</v>
@@ -2419,7 +2437,7 @@
         <v>62</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>63</v>
@@ -2436,13 +2454,13 @@
         <v>64</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F8" s="9">
         <v>7</v>
@@ -2456,13 +2474,13 @@
         <v>67</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F9" s="9">
         <v>1</v>
@@ -2476,13 +2494,13 @@
         <v>70</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F10" s="9">
         <v>1</v>
@@ -2493,22 +2511,22 @@
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B11" s="26" t="s">
+        <v>232</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="D11" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>263</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="F11" s="9" t="s">
+      <c r="G11" s="9" t="s">
         <v>235</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
@@ -2519,7 +2537,7 @@
         <v>74</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>75</v>
@@ -2539,10 +2557,10 @@
         <v>78</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>80</v>
@@ -2553,16 +2571,16 @@
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B14" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>185</v>
-      </c>
       <c r="D14" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
@@ -2575,7 +2593,7 @@
         <v>87</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>88</v>
@@ -2595,7 +2613,7 @@
         <v>92</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>93</v>
@@ -2615,7 +2633,7 @@
         <v>96</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>97</v>
@@ -2635,7 +2653,7 @@
         <v>107</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E18" s="10" t="s">
         <v>48</v>
@@ -2648,10 +2666,10 @@
         <v>108</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E19" s="12" t="s">
         <v>102</v>
@@ -2667,7 +2685,7 @@
         <v>111</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>112</v>
@@ -2683,7 +2701,7 @@
         <v>114</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>112</v>
@@ -2699,7 +2717,7 @@
         <v>116</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E22" s="12" t="s">
         <v>112</v>
@@ -2715,7 +2733,7 @@
         <v>118</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E23" s="12" t="s">
         <v>102</v>
@@ -2731,7 +2749,7 @@
         <v>123</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E24" s="12" t="s">
         <v>121</v>
@@ -2741,13 +2759,13 @@
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B25" s="13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C25" s="12" t="s">
         <v>127</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E25" s="12" t="s">
         <v>105</v>
@@ -2757,13 +2775,13 @@
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B26" s="13" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C26" s="12" t="s">
         <v>129</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E26" s="12" t="s">
         <v>105</v>
@@ -2773,13 +2791,13 @@
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B27" s="13" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C27" s="12" t="s">
         <v>131</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E27" s="12" t="s">
         <v>102</v>
@@ -2789,13 +2807,13 @@
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B28" s="13" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C28" s="12" t="s">
         <v>133</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>134</v>
@@ -2808,10 +2826,10 @@
         <v>135</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E29" s="12" t="s">
         <v>112</v>
@@ -2826,10 +2844,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{974A020C-A60C-4913-8965-C046DA9F3A39}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1048576"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2910,10 +2928,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C7" t="s">
-        <v>174</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -2921,10 +2939,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>173</v>
+        <v>64</v>
       </c>
       <c r="C8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -2932,78 +2950,105 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="C11" t="s">
-        <v>176</v>
+        <v>173</v>
+      </c>
+      <c r="C9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="15">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>274</v>
+      </c>
+      <c r="C10" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C12" t="s">
-        <v>154</v>
+        <v>272</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="15" t="s">
-        <v>139</v>
+      <c r="B13" t="s">
+        <v>270</v>
       </c>
       <c r="C13" t="s">
-        <v>145</v>
+        <v>273</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="C14" t="s">
-        <v>155</v>
+      <c r="B14" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="C15" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
-        <v>177</v>
+        <v>139</v>
       </c>
       <c r="C16" t="s">
-        <v>178</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
-        <v>180</v>
+        <v>140</v>
       </c>
       <c r="C17" t="s">
-        <v>181</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
-        <v>222</v>
+        <v>156</v>
       </c>
       <c r="C18" t="s">
-        <v>223</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
-        <v>224</v>
+        <v>176</v>
       </c>
       <c r="C19" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="C20" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="C21" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="C22" t="s">
         <v>115</v>
       </c>
     </row>
@@ -3016,7 +3061,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A65C4286-6995-4B1C-8EDD-8F561F25CBD8}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -3039,7 +3084,7 @@
         <v>32</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -3050,7 +3095,7 @@
         <v>36</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>37</v>
@@ -3064,7 +3109,7 @@
         <v>43</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>44</v>
@@ -3072,16 +3117,16 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>47</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -3092,7 +3137,7 @@
         <v>52</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>53</v>
@@ -3106,7 +3151,7 @@
         <v>57</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>58</v>
@@ -3120,7 +3165,7 @@
         <v>62</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>63</v>
@@ -3131,13 +3176,13 @@
         <v>64</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -3145,13 +3190,13 @@
         <v>67</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -3159,27 +3204,27 @@
         <v>70</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
+        <v>232</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>234</v>
-      </c>
       <c r="C11" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -3190,7 +3235,7 @@
         <v>74</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>75</v>
@@ -3204,24 +3249,24 @@
         <v>78</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>185</v>
-      </c>
       <c r="C14" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -3232,7 +3277,7 @@
         <v>87</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>88</v>
@@ -3246,7 +3291,7 @@
         <v>92</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>93</v>
@@ -3260,7 +3305,7 @@
         <v>96</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>97</v>
@@ -3268,13 +3313,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D18" s="12" t="s">
         <v>102</v>
@@ -3282,13 +3327,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D19" s="12" t="s">
         <v>102</v>
@@ -3296,13 +3341,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D20" s="12" t="s">
         <v>102</v>
@@ -3310,13 +3355,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D21" s="12" t="s">
         <v>102</v>
@@ -3324,13 +3369,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>102</v>
@@ -3338,69 +3383,69 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D27" s="12" t="s">
         <v>134</v>
@@ -3426,15 +3471,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -3442,7 +3487,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -3450,7 +3495,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -3458,7 +3503,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -3466,7 +3511,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -3474,7 +3519,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -3482,7 +3527,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -3490,7 +3535,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -3498,7 +3543,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -3506,7 +3551,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -3514,7 +3559,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -3522,7 +3567,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B13" s="25">
         <v>4</v>
@@ -3530,7 +3575,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B14" s="25">
         <v>6</v>
@@ -3538,7 +3583,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B15">
         <v>7</v>
@@ -3546,7 +3591,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B16">
         <v>9</v>
@@ -3554,7 +3599,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B17">
         <v>10</v>
@@ -3562,7 +3607,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B18">
         <v>11</v>
@@ -3570,7 +3615,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B19">
         <v>11</v>
@@ -3578,7 +3623,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B20">
         <v>12</v>
@@ -3586,7 +3631,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B21">
         <v>13</v>
@@ -3594,7 +3639,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B22">
         <v>14</v>
@@ -3602,7 +3647,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B23">
         <v>18</v>
@@ -3610,7 +3655,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B24">
         <v>41</v>
@@ -3618,7 +3663,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B25">
         <v>42</v>

</xml_diff>

<commit_message>
Quick calculation of the mass with Simon (2018)
</commit_message>
<xml_diff>
--- a/MINAGRIS_Plastic.R_ReadMe.xlsx
+++ b/MINAGRIS_Plastic.R_ReadMe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berio001\Documents\MINAGRIS_C\MINAGRIS_Microplastic_Soil_Assessmnent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{618273F5-2B62-4F3C-A91B-5ADAE7B1CD52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B45BA00-4512-4391-BCFF-FD57EC2A8220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{A634431C-1F0B-4477-A9DD-2C46E099AE2B}"/>
   </bookViews>
@@ -1656,7 +1656,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1766,8 +1766,8 @@
       <c r="E5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>169</v>
+      <c r="F5" s="28" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -3081,7 +3081,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection sqref="A1:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>